<commit_message>
Cambios realizados: Generación de informes: En la función generar_informes, no filtramos las columnas del DataFrame, por lo que se mantienen todas las columnas originales al exportar los archivos Excel.
Acceso correcto a las filas: En la función emparejar_por_suma, se corrigió el acceso a las filas de la combinación de índices con candidatos.loc[combinacion, 'Debe'].

Con estos cambios, los informes ahora incluirán todas las columnas del archivo original en los archivos punteados.xlsx y no_punteados.xlsx.
</commit_message>
<xml_diff>
--- a/data/Puntear.xlsx
+++ b/data/Puntear.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4A8708-B3B4-4230-8DDC-4BB4BA0AE873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CC02D3-0D8B-4AA9-A46B-48888880F379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Browser" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="47">
   <si>
     <t>F.Mov.</t>
   </si>
@@ -161,18 +161,6 @@
   </si>
   <si>
     <t>409127725/1</t>
-  </si>
-  <si>
-    <t>Compensación Anticipo 409127725/1</t>
-  </si>
-  <si>
-    <t>Creación Anticipo 509014296/1</t>
-  </si>
-  <si>
-    <t>509014296/1</t>
-  </si>
-  <si>
-    <t>Compensación Anticipo 509014296/1</t>
   </si>
 </sst>
 </file>
@@ -561,32 +549,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" customWidth="1"/>
-    <col min="3" max="3" width="34.5546875" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" customWidth="1"/>
-    <col min="5" max="5" width="31.5546875" customWidth="1"/>
-    <col min="6" max="7" width="9.5546875" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
-    <col min="9" max="9" width="4.5546875" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" customWidth="1"/>
-    <col min="11" max="11" width="7.5546875" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" customWidth="1"/>
-    <col min="13" max="13" width="11.5546875" customWidth="1"/>
-    <col min="14" max="14" width="9.5546875" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="6" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -636,7 +624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45581</v>
       </c>
@@ -686,7 +674,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45588</v>
       </c>
@@ -736,7 +724,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45589</v>
       </c>
@@ -786,7 +774,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45600</v>
       </c>
@@ -836,7 +824,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45600</v>
       </c>
@@ -886,7 +874,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45602</v>
       </c>
@@ -936,7 +924,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45602</v>
       </c>
@@ -986,7 +974,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45603</v>
       </c>
@@ -1036,7 +1024,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45607</v>
       </c>
@@ -1086,7 +1074,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45610</v>
       </c>
@@ -1136,7 +1124,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45611</v>
       </c>
@@ -1186,7 +1174,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45611</v>
       </c>
@@ -1236,7 +1224,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45616</v>
       </c>
@@ -1286,7 +1274,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45621</v>
       </c>
@@ -1336,7 +1324,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45631</v>
       </c>
@@ -1386,7 +1374,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45638</v>
       </c>
@@ -1436,7 +1424,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45642</v>
       </c>
@@ -1486,7 +1474,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45656</v>
       </c>
@@ -1534,206 +1522,6 @@
       </c>
       <c r="P19" s="9" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>45665</v>
-      </c>
-      <c r="B20" s="3">
-        <v>5100542</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="5">
-        <v>738.84</v>
-      </c>
-      <c r="G20" s="5">
-        <v>0</v>
-      </c>
-      <c r="H20" s="6">
-        <v>0</v>
-      </c>
-      <c r="I20" s="7">
-        <v>0</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="P20" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>45700</v>
-      </c>
-      <c r="B21" s="3">
-        <v>5104748</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="5">
-        <v>0</v>
-      </c>
-      <c r="G21" s="5">
-        <v>295.91000000000003</v>
-      </c>
-      <c r="H21" s="6">
-        <v>-295.91000000000003</v>
-      </c>
-      <c r="I21" s="7">
-        <v>0</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M21" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="P21" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>45702</v>
-      </c>
-      <c r="B22" s="3">
-        <v>5105413</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="5">
-        <v>67.94</v>
-      </c>
-      <c r="G22" s="5">
-        <v>0</v>
-      </c>
-      <c r="H22" s="6">
-        <v>-227.97</v>
-      </c>
-      <c r="I22" s="7">
-        <v>0</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M22" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="P22" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>45706</v>
-      </c>
-      <c r="B23" s="3">
-        <v>5105965</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="5">
-        <v>83.49</v>
-      </c>
-      <c r="G23" s="5">
-        <v>0</v>
-      </c>
-      <c r="H23" s="6">
-        <v>-144.47999999999999</v>
-      </c>
-      <c r="I23" s="7">
-        <v>0</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N23" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O23" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="P23" s="9" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>